<commit_message>
Ajustes en la descripción de la evaluación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
@@ -461,9 +461,6 @@
     <t>Mapa conceptual del tema La reproducción humana y la sexualidad</t>
   </si>
   <si>
-    <t>Actividad que permite evaluar los conocimientos de los estudiantes acerca del tema La reproducción humana y la sexualidad</t>
-  </si>
-  <si>
     <t>http://recursos.cnice.mec.es/biosfera/alumno/3ESO/apararep/anamasc.htm</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>Actividad que permite conocer la técnica de fecundación in vitro</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos acerca del tema La reproducción humana y la sexualidad</t>
   </si>
 </sst>
 </file>
@@ -1399,42 +1399,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1708,7 +1708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1718,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,94 +1747,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="71" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="Q1" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="71" t="s">
+      <c r="U1" s="77" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="11" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
     </row>
     <row r="3" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -1863,7 +1863,7 @@
         <v>90</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>70</v>
@@ -1920,7 +1920,7 @@
         <v>90</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>70</v>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -1977,7 +1977,7 @@
         <v>91</v>
       </c>
       <c r="J5" s="46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>70</v>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H6" s="16">
         <v>4</v>
@@ -2034,7 +2034,7 @@
         <v>91</v>
       </c>
       <c r="J6" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>70</v>
@@ -2105,19 +2105,19 @@
       <c r="P7" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="81" t="s">
+      <c r="Q7" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="R7" s="82" t="s">
+      <c r="R7" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="S7" s="82" t="s">
+      <c r="S7" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="T7" s="82" t="s">
+      <c r="T7" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="U7" s="83" t="s">
+      <c r="U7" s="73" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2148,7 +2148,7 @@
         <v>91</v>
       </c>
       <c r="J8" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>69</v>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="N8" s="19"/>
       <c r="O8" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P8" s="51" t="s">
         <v>19</v>
@@ -2170,16 +2170,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S8" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S8" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T8" s="70" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H9" s="16">
         <v>7</v>
@@ -2209,7 +2209,7 @@
         <v>91</v>
       </c>
       <c r="J9" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>69</v>
@@ -2229,16 +2229,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S9" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="T9" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="T9" s="70" t="s">
+      <c r="U9" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2268,7 +2268,7 @@
         <v>90</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>70</v>
@@ -2325,7 +2325,7 @@
         <v>91</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>69</v>
@@ -2345,16 +2345,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S11" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S11" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T11" s="70" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H12" s="16">
         <v>10</v>
@@ -2384,7 +2384,7 @@
         <v>91</v>
       </c>
       <c r="J12" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>70</v>
@@ -2439,7 +2439,7 @@
         <v>90</v>
       </c>
       <c r="J13" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>70</v>
@@ -2496,7 +2496,7 @@
         <v>90</v>
       </c>
       <c r="J14" s="46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>70</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H15" s="16">
         <v>13</v>
@@ -2553,7 +2553,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>70</v>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" s="16">
         <v>14</v>
@@ -2606,7 +2606,7 @@
         <v>91</v>
       </c>
       <c r="J16" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>69</v>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P16" s="51" t="s">
         <v>19</v>
@@ -2628,16 +2628,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S16" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S16" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T16" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,7 +2667,7 @@
         <v>91</v>
       </c>
       <c r="J17" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>70</v>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H18" s="16">
         <v>16</v>
@@ -2724,7 +2724,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>70</v>
@@ -2781,7 +2781,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>70</v>
@@ -2795,19 +2795,19 @@
       <c r="P19" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="84" t="s">
+      <c r="Q19" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="R19" s="85" t="s">
+      <c r="R19" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="S19" s="85" t="s">
+      <c r="S19" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="T19" s="85" t="s">
+      <c r="T19" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="U19" s="86" t="s">
+      <c r="U19" s="76" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H21" s="16">
         <v>19</v>
@@ -2895,7 +2895,7 @@
         <v>91</v>
       </c>
       <c r="J21" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>70</v>
@@ -2909,19 +2909,19 @@
       <c r="P21" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="81" t="s">
+      <c r="Q21" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="R21" s="82" t="s">
+      <c r="R21" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="S21" s="82" t="s">
+      <c r="S21" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="T21" s="82" t="s">
+      <c r="T21" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="U21" s="83" t="s">
+      <c r="U21" s="73" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2941,7 +2941,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="14"/>
       <c r="G22" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -2950,7 +2950,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>69</v>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="N22" s="19"/>
       <c r="O22" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P22" s="51" t="s">
         <v>20</v>
@@ -2972,16 +2972,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S22" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S22" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T22" s="70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
       <c r="G23" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H23" s="16">
         <v>21</v>
@@ -3009,7 +3009,7 @@
         <v>91</v>
       </c>
       <c r="J23" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K23" s="17" t="s">
         <v>69</v>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="N23" s="19"/>
       <c r="O23" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P23" s="51" t="s">
         <v>20</v>
@@ -3031,16 +3031,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S23" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S23" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T23" s="70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -3082,19 +3082,19 @@
       <c r="P24" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="84" t="s">
+      <c r="Q24" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="R24" s="85" t="s">
+      <c r="R24" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="S24" s="85" t="s">
+      <c r="S24" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="T24" s="85" t="s">
+      <c r="T24" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="U24" s="86" t="s">
+      <c r="U24" s="76" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3253,7 +3253,7 @@
       <c r="T27" s="24"/>
       <c r="U27" s="27"/>
     </row>
-    <row r="28" spans="1:21" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>67</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="46" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>69</v>
@@ -3298,20 +3298,25 @@
         <v>6</v>
       </c>
       <c r="R28" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S28" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="S28" s="23" t="s">
-        <v>166</v>
-      </c>
       <c r="T28" s="70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3327,11 +3332,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4046,40 +4046,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="77" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="73"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
@@ -4099,10 +4099,10 @@
       </c>
       <c r="F3" s="62"/>
       <c r="G3" s="63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4123,10 +4123,10 @@
       </c>
       <c r="F4" s="29"/>
       <c r="G4" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="65" t="s">
         <v>148</v>
-      </c>
-      <c r="H4" s="65" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4147,10 +4147,10 @@
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="65" t="s">
         <v>150</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4171,10 +4171,10 @@
       </c>
       <c r="F6" s="29"/>
       <c r="G6" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4195,10 +4195,10 @@
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H7" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4219,10 +4219,10 @@
       </c>
       <c r="F8" s="29"/>
       <c r="G8" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H8" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4243,10 +4243,10 @@
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="65" t="s">
         <v>153</v>
-      </c>
-      <c r="H9" s="65" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4267,10 +4267,10 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="65" t="s">
         <v>155</v>
-      </c>
-      <c r="H10" s="65" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4289,10 +4289,10 @@
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H11" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4311,10 +4311,10 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="H12" s="65" t="s">
         <v>158</v>
-      </c>
-      <c r="H12" s="65" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4335,10 +4335,10 @@
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="65" t="s">
         <v>160</v>
-      </c>
-      <c r="H13" s="65" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4359,10 +4359,10 @@
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H14" s="65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4383,10 +4383,10 @@
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H15" s="65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4405,10 +4405,10 @@
       <c r="E16" s="67"/>
       <c r="F16" s="67"/>
       <c r="G16" s="68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" s="69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uso de mayúsculas en escaleta 08-05
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado08\guion05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="15" yWindow="30" windowWidth="10740" windowHeight="11640"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="216">
   <si>
     <t>Asignatura</t>
   </si>
@@ -527,24 +532,6 @@
     <t>Recurso M5A-01</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el sistema reproductor humano</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: el ciclo menstrual</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la gametogénesis</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la reproducción humana</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la fecundación in vitro</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la sexualidad</t>
-  </si>
-  <si>
     <t>Recurso M101A-01</t>
   </si>
   <si>
@@ -678,6 +665,15 @@
   </si>
   <si>
     <t>Mapa conceptual</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El sistema reproductor humano</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La gametogénesis</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La fecundación in vitro</t>
   </si>
 </sst>
 </file>
@@ -1473,13 +1469,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1773,7 +1769,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1783,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,10 +1844,10 @@
       <c r="L1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="88"/>
+      <c r="N1" s="89"/>
       <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
@@ -1875,8 +1871,8 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="86"/>
       <c r="D2" s="86"/>
       <c r="E2" s="86"/>
@@ -1895,11 +1891,11 @@
       </c>
       <c r="O2" s="86"/>
       <c r="P2" s="86"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
     </row>
     <row r="3" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1928,7 +1924,7 @@
         <v>90</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="K3" s="40" t="s">
         <v>70</v>
@@ -1985,7 +1981,7 @@
         <v>90</v>
       </c>
       <c r="J4" s="45" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>70</v>
@@ -2033,7 +2029,7 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -2042,7 +2038,7 @@
         <v>91</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>70</v>
@@ -2090,7 +2086,7 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="H6" s="16">
         <v>4</v>
@@ -2099,7 +2095,7 @@
         <v>91</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>70</v>
@@ -2204,7 +2200,7 @@
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="15" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2213,7 +2209,7 @@
         <v>91</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>69</v>
@@ -2226,7 +2222,7 @@
         <v>22</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="P8" s="50" t="s">
         <v>19</v>
@@ -2241,7 +2237,7 @@
         <v>163</v>
       </c>
       <c r="T8" s="74" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="U8" s="75" t="s">
         <v>165</v>
@@ -2265,7 +2261,7 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="15" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="H9" s="16">
         <v>7</v>
@@ -2274,7 +2270,7 @@
         <v>91</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>69</v>
@@ -2324,7 +2320,7 @@
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="15" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
@@ -2333,7 +2329,7 @@
         <v>91</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>69</v>
@@ -2346,7 +2342,7 @@
         <v>62</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="P10" s="50" t="s">
         <v>19</v>
@@ -2361,7 +2357,7 @@
         <v>163</v>
       </c>
       <c r="T10" s="70" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="U10" s="71" t="s">
         <v>165</v>
@@ -2394,7 +2390,7 @@
         <v>90</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>70</v>
@@ -2451,7 +2447,7 @@
         <v>91</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>69</v>
@@ -2501,7 +2497,7 @@
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="15" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="H13" s="16">
         <v>11</v>
@@ -2510,7 +2506,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>70</v>
@@ -2565,7 +2561,7 @@
         <v>90</v>
       </c>
       <c r="J14" s="45" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>70</v>
@@ -2622,7 +2618,7 @@
         <v>90</v>
       </c>
       <c r="J15" s="45" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>70</v>
@@ -2670,7 +2666,7 @@
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="15" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H16" s="16">
         <v>14</v>
@@ -2679,7 +2675,7 @@
         <v>91</v>
       </c>
       <c r="J16" s="45" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>69</v>
@@ -2692,7 +2688,7 @@
         <v>60</v>
       </c>
       <c r="O16" s="18" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="P16" s="50" t="s">
         <v>20</v>
@@ -2707,7 +2703,7 @@
         <v>163</v>
       </c>
       <c r="T16" s="74" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="U16" s="75" t="s">
         <v>165</v>
@@ -2731,7 +2727,7 @@
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="15" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="H17" s="16">
         <v>15</v>
@@ -2740,7 +2736,7 @@
         <v>91</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>70</v>
@@ -2797,7 +2793,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>70</v>
@@ -2845,7 +2841,7 @@
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="15" t="s">
-        <v>172</v>
+        <v>215</v>
       </c>
       <c r="H19" s="16">
         <v>17</v>
@@ -2854,7 +2850,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>70</v>
@@ -2911,7 +2907,7 @@
         <v>90</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>69</v>
@@ -2924,7 +2920,7 @@
       </c>
       <c r="N20" s="19"/>
       <c r="O20" s="18" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="P20" s="50" t="s">
         <v>19</v>
@@ -2933,16 +2929,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="80" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="S20" s="80" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="T20" s="80" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="U20" s="81" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2972,7 +2968,7 @@
         <v>91</v>
       </c>
       <c r="J21" s="45" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>70</v>
@@ -3016,11 +3012,11 @@
         <v>127</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="15" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -3029,7 +3025,7 @@
         <v>90</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>69</v>
@@ -3042,7 +3038,7 @@
       </c>
       <c r="N22" s="19"/>
       <c r="O22" s="18" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="P22" s="50" t="s">
         <v>19</v>
@@ -3051,16 +3047,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="80" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="S22" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="T22" s="80" t="s">
         <v>209</v>
       </c>
-      <c r="T22" s="80" t="s">
-        <v>215</v>
-      </c>
       <c r="U22" s="81" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3114,7 +3110,7 @@
         <v>101</v>
       </c>
       <c r="T23" s="77" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="U23" s="78" t="s">
         <v>102</v>
@@ -3138,7 +3134,7 @@
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="15" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="H24" s="16">
         <v>22</v>
@@ -3147,7 +3143,7 @@
         <v>91</v>
       </c>
       <c r="J24" s="45" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>70</v>
@@ -3358,7 +3354,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="14"/>
       <c r="G28" s="15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3412,7 +3408,7 @@
         <v>91</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>69</v>
@@ -3460,7 +3456,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="14"/>
       <c r="G30" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H30" s="16">
         <v>28</v>
@@ -3469,7 +3465,7 @@
         <v>91</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>69</v>
@@ -3495,7 +3491,7 @@
         <v>163</v>
       </c>
       <c r="T30" s="74" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="U30" s="75" t="s">
         <v>165</v>
@@ -3503,11 +3499,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3523,6 +3514,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4263,14 +4259,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="95"/>
-      <c r="H2" s="89"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">

</xml_diff>

<commit_message>
Corrección de la descripción de un recurso
El REC160 estaba como actividad cuando es interactivo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="VER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="217">
   <si>
     <t>Asignatura</t>
   </si>
@@ -590,9 +590,6 @@
     <t>Actividad para repasar los conceptos asociados a la reproducción humana</t>
   </si>
   <si>
-    <t>Actividad que permite conocer la técnica de fecundación in vitro</t>
-  </si>
-  <si>
     <t>Evalúa tus conocimientos acerca del tema La reproducción humana y la sexualidad</t>
   </si>
   <si>
@@ -672,6 +669,9 @@
   </si>
   <si>
     <t>Cambiar acento</t>
+  </si>
+  <si>
+    <t>Interactivo con animación incluida que permite conocer la técnica de fecundación in vitro</t>
   </si>
 </sst>
 </file>
@@ -1467,13 +1467,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1767,7 +1767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1778,7 +1778,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,10 +1842,10 @@
       <c r="L1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="M1" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="89"/>
+      <c r="N1" s="88"/>
       <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
@@ -1869,8 +1869,8 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="86"/>
       <c r="D2" s="86"/>
       <c r="E2" s="86"/>
@@ -1889,11 +1889,11 @@
       </c>
       <c r="O2" s="86"/>
       <c r="P2" s="86"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="89"/>
     </row>
     <row r="3" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1933,7 +1933,7 @@
       <c r="M3" s="42"/>
       <c r="N3" s="42"/>
       <c r="O3" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P3" s="49" t="s">
         <v>19</v>
@@ -1992,7 +1992,7 @@
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
       <c r="O4" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P4" s="50" t="s">
         <v>19</v>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H6" s="16">
         <v>4</v>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2211,7 +2211,7 @@
         <v>91</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>69</v>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H9" s="16">
         <v>7</v>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
@@ -2344,7 +2344,7 @@
         <v>62</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P10" s="50" t="s">
         <v>19</v>
@@ -2403,7 +2403,7 @@
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P11" s="50" t="s">
         <v>19</v>
@@ -2633,7 +2633,7 @@
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
       <c r="O15" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P15" s="50" t="s">
         <v>19</v>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H16" s="16">
         <v>14</v>
@@ -2796,20 +2796,22 @@
         <v>16</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>70</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="18"/>
+      <c r="O18" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="P18" s="50" t="s">
         <v>19</v>
       </c>
@@ -2847,7 +2849,7 @@
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H19" s="16">
         <v>17</v>
@@ -2913,7 +2915,7 @@
         <v>90</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>69</v>
@@ -2926,7 +2928,7 @@
       </c>
       <c r="N20" s="19"/>
       <c r="O20" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P20" s="50" t="s">
         <v>19</v>
@@ -2935,16 +2937,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="80" t="s">
+        <v>200</v>
+      </c>
+      <c r="S20" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="S20" s="80" t="s">
+      <c r="T20" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="T20" s="80" t="s">
+      <c r="U20" s="81" t="s">
         <v>203</v>
-      </c>
-      <c r="U20" s="81" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3018,11 +3020,11 @@
         <v>127</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -3031,7 +3033,7 @@
         <v>90</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>69</v>
@@ -3044,7 +3046,7 @@
       </c>
       <c r="N22" s="19"/>
       <c r="O22" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P22" s="50" t="s">
         <v>19</v>
@@ -3053,16 +3055,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="80" t="s">
+        <v>200</v>
+      </c>
+      <c r="S22" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="S22" s="80" t="s">
-        <v>202</v>
-      </c>
       <c r="T22" s="80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U22" s="81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3116,7 +3118,7 @@
         <v>101</v>
       </c>
       <c r="T23" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U23" s="78" t="s">
         <v>102</v>
@@ -3360,7 +3362,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="14"/>
       <c r="G28" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3414,7 +3416,7 @@
         <v>91</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>69</v>
@@ -3462,7 +3464,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="14"/>
       <c r="G30" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H30" s="16">
         <v>28</v>
@@ -3471,7 +3473,7 @@
         <v>91</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>69</v>
@@ -3497,7 +3499,7 @@
         <v>163</v>
       </c>
       <c r="T30" s="74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U30" s="75" t="s">
         <v>165</v>
@@ -3505,6 +3507,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3520,11 +3527,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4265,14 +4267,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
       <c r="G2" s="95"/>
-      <c r="H2" s="87"/>
+      <c r="H2" s="89"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">

</xml_diff>

<commit_message>
CN0706, CN0805, CN0807 y CN0806: Escaletas y esqueletos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion05/ESCALETA_CN_08_05_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="30" windowWidth="10740" windowHeight="11640"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="10740" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="ESCALETA" sheetId="1" r:id="rId1"/>
@@ -1467,13 +1467,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1767,7 +1767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1777,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,14 +1794,14 @@
     <col min="10" max="10" width="92.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="14" style="5" customWidth="1"/>
-    <col min="15" max="15" width="27.7109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="3" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" customWidth="1"/>
     <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.7109375" customWidth="1"/>
+    <col min="20" max="20" width="37.42578125" customWidth="1"/>
     <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1842,10 +1842,10 @@
       <c r="L1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="88"/>
+      <c r="N1" s="89"/>
       <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
@@ -1869,8 +1869,8 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="86"/>
       <c r="D2" s="86"/>
       <c r="E2" s="86"/>
@@ -1889,11 +1889,11 @@
       </c>
       <c r="O2" s="86"/>
       <c r="P2" s="86"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
     </row>
     <row r="3" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -3507,11 +3507,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3527,6 +3522,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4267,14 +4267,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="95"/>
-      <c r="H2" s="89"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">

</xml_diff>